<commit_message>
Fixed Project 1 Presentation
Fixed project 1 presentation so that fewer
slides exist in the main presentation.
All slides with methodology in them
are now in the slide backups.
</commit_message>
<xml_diff>
--- a/Project-1-Post-Processing-of-Hadoop-Results.xlsx
+++ b/Project-1-Post-Processing-of-Hadoop-Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Question1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="484">
   <si>
     <t>Year</t>
   </si>
@@ -1459,12 +1459,6 @@
   </si>
   <si>
     <t>Region Name</t>
-  </si>
-  <si>
-    <t>PUT CHART TITLE IN PPT SLIDE ABOVE THE CHART!</t>
-  </si>
-  <si>
-    <t>PUT THE TABLE IN COLUMNS A THROUGH D IN THE PPT SLIDE BACKUPS!</t>
   </si>
   <si>
     <t>Micronesia - Fed. Sts.</t>
@@ -1566,7 +1560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1620,8 +1614,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1918,11 +1913,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168137472"/>
-        <c:axId val="168139392"/>
+        <c:axId val="185168640"/>
+        <c:axId val="185170560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168137472"/>
+        <c:axId val="185168640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168139392"/>
+        <c:crossAx val="185170560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1963,7 +1958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168139392"/>
+        <c:axId val="185170560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1992,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168137472"/>
+        <c:crossAx val="185168640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,11 +2182,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="168073856"/>
-        <c:axId val="168079744"/>
+        <c:axId val="185371264"/>
+        <c:axId val="185373056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168073856"/>
+        <c:axId val="185371264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2016"/>
@@ -2203,13 +2198,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168079744"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="185373056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168079744"/>
+        <c:axId val="185373056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.2000000000000002"/>
@@ -2245,7 +2250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168073856"/>
+        <c:crossAx val="185371264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2433,11 +2438,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="168780160"/>
-        <c:axId val="168781696"/>
+        <c:axId val="185422208"/>
+        <c:axId val="185423744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168780160"/>
+        <c:axId val="185422208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2016"/>
@@ -2450,7 +2455,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="60000"/>
+          <a:bodyPr rot="-5400000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2459,13 +2464,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168781696"/>
+        <c:crossAx val="185423744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168781696"/>
+        <c:axId val="185423744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -2501,7 +2506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168780160"/>
+        <c:crossAx val="185422208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2689,11 +2694,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="168808448"/>
-        <c:axId val="168809984"/>
+        <c:axId val="185454592"/>
+        <c:axId val="185456128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168808448"/>
+        <c:axId val="185454592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2016"/>
@@ -2715,13 +2720,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168809984"/>
+        <c:crossAx val="185456128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168809984"/>
+        <c:axId val="185456128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-2.5"/>
@@ -2756,7 +2761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168808448"/>
+        <c:crossAx val="185454592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2946,11 +2951,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="17052800"/>
-        <c:axId val="17054336"/>
+        <c:axId val="185542144"/>
+        <c:axId val="185543680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17052800"/>
+        <c:axId val="185542144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2016"/>
@@ -2972,13 +2977,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17054336"/>
+        <c:crossAx val="185543680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17054336"/>
+        <c:axId val="185543680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,7 +3017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="17052800"/>
+        <c:crossAx val="185542144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -3273,11 +3278,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168754176"/>
-        <c:axId val="168166528"/>
+        <c:axId val="185555584"/>
+        <c:axId val="185500416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168754176"/>
+        <c:axId val="185555584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3310,7 +3315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168166528"/>
+        <c:crossAx val="185500416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3318,7 +3323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168166528"/>
+        <c:axId val="185500416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3360,7 +3365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168754176"/>
+        <c:crossAx val="185555584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -3601,11 +3606,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168153472"/>
-        <c:axId val="168155392"/>
+        <c:axId val="184790016"/>
+        <c:axId val="185566336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168153472"/>
+        <c:axId val="184790016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3638,7 +3643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168155392"/>
+        <c:crossAx val="185566336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3646,7 +3651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168155392"/>
+        <c:axId val="185566336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3688,7 +3693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168153472"/>
+        <c:crossAx val="184790016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -3782,10 +3787,10 @@
       <xdr:rowOff>487680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3806,16 +3811,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>472440</xdr:rowOff>
+      <xdr:rowOff>236220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3838,16 +3843,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>472440</xdr:rowOff>
+      <xdr:rowOff>487680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3870,16 +3875,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>480060</xdr:rowOff>
+      <xdr:rowOff>502920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4621,11 +4626,9 @@
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
-      <c r="N1" s="18" t="s">
-        <v>479</v>
-      </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5899,9 +5902,8 @@
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="I1:L1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11657,7 +11659,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N163"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11690,11 +11692,9 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
-      <c r="L1" s="21" t="s">
-        <v>478</v>
-      </c>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -14679,9 +14679,8 @@
       <sortCondition descending="1" ref="E1:E163"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14692,7 +14691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14705,32 +14704,32 @@
   <sheetData>
     <row r="1" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="18" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C1" s="18"/>
       <c r="F1" s="18" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>483</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>483</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -15224,7 +15223,7 @@
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F27" s="15">
         <v>7</v>
@@ -15675,7 +15674,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B50" s="15">
         <v>36</v>

</xml_diff>